<commit_message>
validate data with BS4
</commit_message>
<xml_diff>
--- a/EgyptProPlayers.xlsx
+++ b/EgyptProPlayers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,74 +456,202 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Mohamed Salah</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>&lt;selenium.webdriver.remote.webelement.WebElement (session="541bdf554c95d4ec6759000e3075b0d5", element="e3a0dd41-3bf8-4dac-8f8e-5d3d416a4786")&gt;</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Karim Hafez</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>&lt;selenium.webdriver.remote.webelement.WebElement (session="541bdf554c95d4ec6759000e3075b0d5", element="37507a99-8716-466e-8f8f-c85c5b259f5e")&gt;</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mostafa Mohamed</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>&lt;selenium.webdriver.remote.webelement.WebElement (session="541bdf554c95d4ec6759000e3075b0d5", element="b78f6376-7abb-4f42-8107-fd660a8fed0a")&gt;</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Trezeguet</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>&lt;selenium.webdriver.remote.webelement.WebElement (session="541bdf554c95d4ec6759000e3075b0d5", element="c12aa96f-a703-43ce-9093-c9678070fd4d")&gt;</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Mohamed Elneny</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>&lt;selenium.webdriver.remote.webelement.WebElement (session="541bdf554c95d4ec6759000e3075b0d5", element="878f7582-a443-4019-a9b5-74adbb9ae3b7")&gt;</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Omar Marmoush</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>&lt;selenium.webdriver.remote.webelement.WebElement (session="541bdf554c95d4ec6759000e3075b0d5", element="13d028e9-a42b-4ab9-b0f8-305b125ff142")&gt;</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ahmed Hegazy</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>&lt;selenium.webdriver.remote.webelement.WebElement (session="541bdf554c95d4ec6759000e3075b0d5", element="c7493cd3-1127-40c0-88bf-38ea1533f35a")&gt;</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ahmed Elmohamady</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Salah Basha</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>